<commit_message>
fix deceleration problem - change unsigned to signed
</commit_message>
<xml_diff>
--- a/esp32_divider.xlsx
+++ b/esp32_divider.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\privat\penplotter_04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C8B011-4F25-49AA-8BFD-55134FE5E5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B699DD2-CBFF-46B5-8F12-0771D1240017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30570" yWindow="720" windowWidth="26670" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="1020" windowWidth="26670" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -156,11 +156,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -455,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +471,8 @@
     <col min="11" max="11" width="9.42578125" customWidth="1"/>
     <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.28515625" customWidth="1"/>
+    <col min="18" max="18" width="23" customWidth="1"/>
+    <col min="19" max="19" width="16.28515625" customWidth="1"/>
     <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="34.42578125" customWidth="1"/>
     <col min="23" max="24" width="15" customWidth="1"/>
@@ -507,16 +509,16 @@
         <v>200</v>
       </c>
       <c r="Q3">
-        <v>114720</v>
+        <v>16000</v>
       </c>
       <c r="R3">
-        <v>1114.95</v>
+        <v>3388705</v>
       </c>
       <c r="S3">
-        <v>4459.8</v>
+        <v>564784</v>
       </c>
       <c r="T3">
-        <v>41157040</v>
+        <v>8094114</v>
       </c>
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.25">
@@ -530,11 +532,11 @@
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q6">
         <f>(S3-R3)*2000000 / T3</f>
-        <v>162.54084355920642</v>
-      </c>
-      <c r="R6">
+        <v>-697771.49172843376</v>
+      </c>
+      <c r="R6" s="4">
         <f>R3*R3</f>
-        <v>1243113.5025000002</v>
+        <v>11483321577025</v>
       </c>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
@@ -618,12 +620,12 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <f>SQRT($Q$6 * Q10 + $R$6)</f>
-        <v>1114.95</v>
+        <f>SQRT($Q$6 * Q10 * 1000 + $R$6)</f>
+        <v>3388705</v>
       </c>
       <c r="S10">
         <f>10000000/R10</f>
-        <v>8969.0120633212246</v>
+        <v>2.9509797990677855</v>
       </c>
       <c r="Y10" s="2"/>
     </row>
@@ -670,15 +672,15 @@
       </c>
       <c r="Q11">
         <f>$Q$3*P11</f>
-        <v>11472</v>
+        <v>1600</v>
       </c>
       <c r="R11">
-        <f>SQRT($Q$6 * Q11 + $R$6)</f>
-        <v>1762.8902574497417</v>
+        <f t="shared" ref="R11:R20" si="8">SQRT($Q$6 * Q11 * 1000 + $R$6)</f>
+        <v>3219765.0830859547</v>
       </c>
       <c r="S11">
-        <f t="shared" ref="S11:S20" si="8">10000000/R11</f>
-        <v>5672.5028445425451</v>
+        <f t="shared" ref="S11:S20" si="9">10000000/R11</f>
+        <v>3.1058166487151264</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
@@ -696,14 +698,14 @@
         <v>0.1</v>
       </c>
       <c r="G12">
-        <f t="shared" ref="G12" si="9">(F12/40)*360</f>
+        <f t="shared" ref="G12" si="10">(F12/40)*360</f>
         <v>0.9</v>
       </c>
       <c r="I12">
         <v>32</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12" si="10">G12*I12*400/360</f>
+        <f t="shared" ref="J12" si="11">G12*I12*400/360</f>
         <v>32</v>
       </c>
       <c r="K12">
@@ -719,20 +721,20 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <f t="shared" ref="P12:P20" si="11">P11+0.1</f>
+        <f t="shared" ref="P12:P20" si="12">P11+0.1</f>
         <v>0.2</v>
       </c>
       <c r="Q12">
-        <f t="shared" ref="Q12:Q20" si="12">$Q$3*P12</f>
-        <v>22944</v>
+        <f t="shared" ref="Q12:Q20" si="13">$Q$3*P12</f>
+        <v>3200</v>
       </c>
       <c r="R12">
-        <f t="shared" ref="R12:R20" si="13">SQRT($Q$6 * Q12 + $R$6)</f>
-        <v>2229.8992392308742</v>
+        <f t="shared" si="8"/>
+        <v>3041455.704673999</v>
       </c>
       <c r="S12">
-        <f t="shared" si="8"/>
-        <v>4484.5075616282784</v>
+        <f t="shared" si="9"/>
+        <v>3.2878992729147303</v>
       </c>
       <c r="V12" s="3"/>
     </row>
@@ -774,20 +776,20 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="12"/>
-        <v>34416.000000000007</v>
+        <f t="shared" si="13"/>
+        <v>4800.0000000000009</v>
       </c>
       <c r="R13">
-        <f t="shared" si="13"/>
-        <v>2614.7885525284159</v>
+        <f t="shared" si="8"/>
+        <v>2852020.0589632108</v>
       </c>
       <c r="S13">
-        <f t="shared" si="8"/>
-        <v>3824.4010171798877</v>
+        <f t="shared" si="9"/>
+        <v>3.5062866996928768</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
@@ -828,20 +830,20 @@
         <v>0</v>
       </c>
       <c r="P14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.4</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="12"/>
-        <v>45888</v>
+        <f t="shared" si="13"/>
+        <v>6400</v>
       </c>
       <c r="R14">
-        <f t="shared" si="13"/>
-        <v>2949.8792740966305</v>
+        <f t="shared" si="8"/>
+        <v>2649072.2960997163</v>
       </c>
       <c r="S14">
-        <f t="shared" si="8"/>
-        <v>3389.9692396945279</v>
+        <f t="shared" si="9"/>
+        <v>3.7749064133595773</v>
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
@@ -882,20 +884,20 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="12"/>
-        <v>57360</v>
+        <f t="shared" si="13"/>
+        <v>8000</v>
       </c>
       <c r="R15">
-        <f t="shared" si="13"/>
-        <v>3250.6086028705577</v>
+        <f t="shared" si="8"/>
+        <v>2429228.199078368</v>
       </c>
       <c r="S15">
-        <f t="shared" si="8"/>
-        <v>3076.3469927351971</v>
+        <f t="shared" si="9"/>
+        <v>4.1165338043556092</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
@@ -936,20 +938,20 @@
         <v>3.0719016991497483E-2</v>
       </c>
       <c r="P16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="12"/>
-        <v>68832</v>
+        <f t="shared" si="13"/>
+        <v>9600</v>
       </c>
       <c r="R16">
-        <f>SQRT($Q$6 * Q16 + $R$6)</f>
-        <v>3525.7800337467588</v>
+        <f t="shared" si="8"/>
+        <v>2187399.1991477082</v>
       </c>
       <c r="S16">
-        <f t="shared" si="8"/>
-        <v>2836.2518093260765</v>
+        <f t="shared" si="9"/>
+        <v>4.571639234345688</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
@@ -990,20 +992,20 @@
         <v>8.1914757455479048E-2</v>
       </c>
       <c r="P17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.7</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="12"/>
-        <v>80304</v>
+        <f t="shared" si="13"/>
+        <v>11200</v>
       </c>
       <c r="R17">
-        <f t="shared" si="13"/>
-        <v>3780.9778369726678</v>
+        <f t="shared" si="8"/>
+        <v>1915275.6641451227</v>
       </c>
       <c r="S17">
-        <f t="shared" si="8"/>
-        <v>2644.8184652694881</v>
+        <f t="shared" si="9"/>
+        <v>5.2211805262316995</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
@@ -1044,20 +1046,20 @@
         <v>0</v>
       </c>
       <c r="P18">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="12"/>
-        <v>91775.999999999985</v>
+        <f t="shared" si="13"/>
+        <v>12799.999999999998</v>
       </c>
       <c r="R18">
-        <f t="shared" si="13"/>
-        <v>4020.0077065833748</v>
+        <f t="shared" si="8"/>
+        <v>1597449.993865551</v>
       </c>
       <c r="S18">
-        <f t="shared" si="8"/>
-        <v>2487.5574202565526</v>
+        <f t="shared" si="9"/>
+        <v>6.2599768621249545</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -1098,20 +1100,20 @@
         <v>0</v>
       </c>
       <c r="P19">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="12"/>
-        <v>103247.99999999999</v>
+        <f t="shared" si="13"/>
+        <v>14399.999999999998</v>
       </c>
       <c r="R19">
-        <f t="shared" si="13"/>
-        <v>4245.6013141015655</v>
+        <f t="shared" si="8"/>
+        <v>1198086.8483275971</v>
       </c>
       <c r="S19">
-        <f t="shared" si="8"/>
-        <v>2355.3789581667666</v>
+        <f t="shared" si="9"/>
+        <v>8.3466403240791305</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
@@ -1152,20 +1154,20 @@
         <v>-0.76812289966437675</v>
       </c>
       <c r="P20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="12"/>
-        <v>114719.99999999999</v>
+        <f t="shared" si="13"/>
+        <v>15999.999999999998</v>
       </c>
       <c r="R20">
-        <f t="shared" si="13"/>
-        <v>4459.7980980771044</v>
+        <f t="shared" si="8"/>
+        <v>564781.11633628525</v>
       </c>
       <c r="S20">
-        <f t="shared" si="8"/>
-        <v>2242.2539720602194</v>
+        <f t="shared" si="9"/>
+        <v>17.705974422214467</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">

</xml_diff>